<commit_message>
Se arregló el problema de las imágenes que no se enviaban en el cuerpo del correo
</commit_message>
<xml_diff>
--- a/files/emails.xlsx
+++ b/files/emails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sopor\Documents\script_py\sendEmail\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F8E8E8-4016-4354-8582-C68A28FCEFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EC404C-C6B8-4056-8A87-30E1022A94EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1476" yWindow="1620" windowWidth="17304" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -64,6 +64,30 @@
   </si>
   <si>
     <t>Mensaje</t>
+  </si>
+  <si>
+    <t>Julianaslvth@gmail.com</t>
+  </si>
+  <si>
+    <t>Juliana Gironza</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Innverto</t>
+  </si>
+  <si>
+    <t>Comercial@innverto.com</t>
+  </si>
+  <si>
+    <t>Info@innverto.com</t>
+  </si>
+  <si>
+    <t>Sebastián Zapata</t>
+  </si>
+  <si>
+    <t>sebastiandzr@live.com</t>
   </si>
 </sst>
 </file>
@@ -108,9 +132,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -392,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,12 +484,84 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{30350148-156D-4FA0-B96B-EDBF623671E0}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{F2759544-9BB9-4060-B6AD-329553D1AF0F}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{C6029371-13AA-4781-8278-79FCA6654F02}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{8B39D0A5-6B32-40A0-BE90-45AB05AA3DD8}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{09FAEEAE-6869-4D54-8F75-C313EB313753}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{145BDD07-C23D-428C-9C4E-FB347AD97B6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>